<commit_message>
Updates.. Fetching Forex from CSI
</commit_message>
<xml_diff>
--- a/Auto/ASSETS.xlsx
+++ b/Auto/ASSETS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trading\Auto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0C649F-6B24-40A6-86D1-5A2D13DC262E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03547E63-FE64-4446-A14C-B28E5C3530B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7950" yWindow="2730" windowWidth="16875" windowHeight="10470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSETS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="141">
   <si>
     <t>symbol</t>
   </si>
@@ -346,12 +346,6 @@
     <t>Cotton</t>
   </si>
   <si>
-    <t>IB</t>
-  </si>
-  <si>
-    <t>IG</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -374,6 +368,81 @@
   </si>
   <si>
     <t>5Y Treasury</t>
+  </si>
+  <si>
+    <t>SEF</t>
+  </si>
+  <si>
+    <t>AD6</t>
+  </si>
+  <si>
+    <t>DR5</t>
+  </si>
+  <si>
+    <t>EU9</t>
+  </si>
+  <si>
+    <t>QE2</t>
+  </si>
+  <si>
+    <t>QE9</t>
+  </si>
+  <si>
+    <t>QE_</t>
+  </si>
+  <si>
+    <t>QE{</t>
+  </si>
+  <si>
+    <t>QE}</t>
+  </si>
+  <si>
+    <t>QF3</t>
+  </si>
+  <si>
+    <t>US5</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>USDAUD</t>
+  </si>
+  <si>
+    <t>USDEUR</t>
+  </si>
+  <si>
+    <t>USDCAD</t>
+  </si>
+  <si>
+    <t>USDJPY</t>
+  </si>
+  <si>
+    <t>USDZAR</t>
+  </si>
+  <si>
+    <t>USDSGD</t>
+  </si>
+  <si>
+    <t>USDCHF</t>
+  </si>
+  <si>
+    <t>USDKRW</t>
+  </si>
+  <si>
+    <t>USDGBP</t>
+  </si>
+  <si>
+    <t>USDBRL</t>
+  </si>
+  <si>
+    <t>USDINR</t>
+  </si>
+  <si>
+    <t>FX</t>
+  </si>
+  <si>
+    <t>ticker</t>
   </si>
 </sst>
 </file>
@@ -930,17 +999,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J51" totalsRowShown="0">
-  <autoFilter ref="A1:J51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I62" totalsRowShown="0">
+  <autoFilter ref="A1:I62" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I51">
+    <sortCondition ref="D2:D51"/>
     <sortCondition ref="E2:E51"/>
-    <sortCondition ref="F2:F51"/>
     <sortCondition ref="A2:A51"/>
   </sortState>
-  <tableColumns count="10">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="symbol"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="IB" dataDxfId="0"/>
-    <tableColumn id="12" xr3:uid="{752A0812-CAC3-44D8-8FC2-359BA34AFC6E}" name="IG"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="ticker" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="group"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="secType"/>
@@ -1250,1507 +1318,1713 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="8.53125" customWidth="1"/>
-    <col min="4" max="4" width="15.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.9296875" customWidth="1"/>
-    <col min="6" max="6" width="9.1328125" customWidth="1"/>
-    <col min="7" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="9.59765625" customWidth="1"/>
-    <col min="10" max="10" width="10.53125" customWidth="1"/>
+    <col min="1" max="2" width="8.53125" customWidth="1"/>
+    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.9296875" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" customWidth="1"/>
+    <col min="6" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="9.59765625" customWidth="1"/>
+    <col min="9" max="9" width="10.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
         <v>55</v>
       </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
-        <v>102</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
       </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="H4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="H5" t="s">
-        <v>102</v>
-      </c>
-      <c r="I5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="H6" t="s">
-        <v>102</v>
-      </c>
-      <c r="I6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="H7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>84</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="H8" t="s">
-        <v>102</v>
-      </c>
-      <c r="I8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>86</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="H10" t="s">
-        <v>102</v>
-      </c>
-      <c r="I10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="I10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>96</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" t="s">
         <v>93</v>
       </c>
-      <c r="J11">
+      <c r="I11">
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>77</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="H12" t="s">
-        <v>102</v>
-      </c>
-      <c r="I12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12">
+        <v>9</v>
+      </c>
+      <c r="I12">
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" t="s">
+        <v>107</v>
+      </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="H13" t="s">
-        <v>102</v>
-      </c>
-      <c r="I13" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13">
+        <v>9</v>
+      </c>
+      <c r="I13">
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>103</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="H14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="I14">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>90</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" t="s">
         <v>93</v>
       </c>
-      <c r="J15">
+      <c r="I15">
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>89</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I16" t="s">
         <v>93</v>
       </c>
-      <c r="J16">
+      <c r="I16">
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>94</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" t="s">
+        <v>95</v>
+      </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
-      </c>
-      <c r="I17" t="s">
         <v>93</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>75</v>
       </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" t="s">
         <v>93</v>
       </c>
-      <c r="J18">
+      <c r="I18">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>65</v>
       </c>
       <c r="B19" t="s">
         <v>74</v>
       </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
-      </c>
-      <c r="I19" t="s">
         <v>93</v>
       </c>
-      <c r="J19">
+      <c r="I19">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>59</v>
       </c>
       <c r="B20" t="s">
         <v>59</v>
       </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>70</v>
-      </c>
-      <c r="I20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20">
+        <v>9</v>
+      </c>
+      <c r="I20">
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G21" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="H21" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21">
+        <v>9</v>
+      </c>
+      <c r="I21">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>60</v>
       </c>
       <c r="B22" t="s">
         <v>60</v>
       </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="H22" t="s">
-        <v>70</v>
-      </c>
-      <c r="I22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22">
+        <v>9</v>
+      </c>
+      <c r="I22">
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>57</v>
       </c>
       <c r="B23" t="s">
         <v>57</v>
       </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="H23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I23" t="s">
-        <v>9</v>
-      </c>
-      <c r="J23">
+        <v>9</v>
+      </c>
+      <c r="I23">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>78</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="H24" t="s">
-        <v>102</v>
-      </c>
-      <c r="I24" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24">
+        <v>9</v>
+      </c>
+      <c r="I24">
         <v>42000</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
       </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F25" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="H25" t="s">
-        <v>72</v>
-      </c>
-      <c r="I25" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25">
+        <v>9</v>
+      </c>
+      <c r="I25">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>100</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
       <c r="D26" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F26" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G26" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="H26" t="s">
-        <v>72</v>
-      </c>
-      <c r="I26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s">
         <v>16</v>
       </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
         <v>63</v>
       </c>
-      <c r="F27" t="s">
+      <c r="E28" t="s">
         <v>18</v>
       </c>
-      <c r="G27" t="s">
+      <c r="F28" t="s">
         <v>19</v>
       </c>
-      <c r="H27" t="s">
-        <v>102</v>
-      </c>
-      <c r="I27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="G28" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>112</v>
       </c>
-      <c r="E28" t="s">
+      <c r="B29" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" t="s">
         <v>63</v>
       </c>
-      <c r="F28" t="s">
+      <c r="E29" t="s">
         <v>18</v>
       </c>
-      <c r="G28" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" t="s">
-        <v>102</v>
-      </c>
-      <c r="I28" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" s="2">
+      <c r="G29" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C30" t="s">
         <v>115</v>
       </c>
-      <c r="E29" t="s">
+      <c r="D30" t="s">
         <v>63</v>
       </c>
-      <c r="F29" t="s">
+      <c r="E30" t="s">
         <v>18</v>
       </c>
-      <c r="H29" t="s">
-        <v>102</v>
-      </c>
-      <c r="I29" t="s">
-        <v>9</v>
-      </c>
-      <c r="J29" s="2">
+      <c r="G30" t="s">
+        <v>102</v>
+      </c>
+      <c r="H30" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" t="s">
-        <v>102</v>
-      </c>
-      <c r="I30" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
       <c r="D31" t="s">
         <v>33</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G31" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H31" t="s">
-        <v>102</v>
-      </c>
-      <c r="I31" t="s">
-        <v>9</v>
-      </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
       <c r="D32" t="s">
         <v>33</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G32" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H32" t="s">
-        <v>102</v>
-      </c>
-      <c r="I32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
       <c r="D33" t="s">
         <v>33</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F33" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G33" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H33" t="s">
-        <v>102</v>
-      </c>
-      <c r="I33" t="s">
-        <v>9</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
       <c r="D34" t="s">
         <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G34" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H34" t="s">
-        <v>102</v>
-      </c>
-      <c r="I34" t="s">
-        <v>9</v>
-      </c>
-      <c r="J34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>38</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
       <c r="D35" t="s">
         <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F35" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G35" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H35" t="s">
-        <v>102</v>
-      </c>
-      <c r="I35" t="s">
-        <v>9</v>
-      </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>39</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
       <c r="D36" t="s">
         <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G36" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H36" t="s">
-        <v>102</v>
-      </c>
-      <c r="I36" t="s">
-        <v>9</v>
-      </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>40</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
       </c>
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
       <c r="D37" t="s">
         <v>33</v>
       </c>
       <c r="E37" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F37" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G37" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H37" t="s">
-        <v>102</v>
-      </c>
-      <c r="I37" t="s">
-        <v>9</v>
-      </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>41</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
       <c r="D38" t="s">
         <v>33</v>
       </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G38" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H38" t="s">
-        <v>102</v>
-      </c>
-      <c r="I38" t="s">
-        <v>9</v>
-      </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>42</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
       </c>
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
       <c r="D39" t="s">
         <v>33</v>
       </c>
       <c r="E39" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G39" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H39" t="s">
-        <v>102</v>
-      </c>
-      <c r="I39" t="s">
-        <v>9</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>43</v>
       </c>
       <c r="B40" t="s">
         <v>43</v>
       </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
       <c r="D40" t="s">
         <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F40" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G40" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H40" t="s">
-        <v>102</v>
-      </c>
-      <c r="I40" t="s">
-        <v>9</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>44</v>
       </c>
       <c r="B41" t="s">
         <v>44</v>
       </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
       <c r="D41" t="s">
         <v>33</v>
       </c>
       <c r="E41" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F41" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G41" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H41" t="s">
-        <v>102</v>
-      </c>
-      <c r="I41" t="s">
-        <v>9</v>
-      </c>
-      <c r="J41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>45</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
       </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
       <c r="D42" t="s">
         <v>33</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G42" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H42" t="s">
-        <v>102</v>
-      </c>
-      <c r="I42" t="s">
-        <v>9</v>
-      </c>
-      <c r="J42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>46</v>
       </c>
       <c r="B43" t="s">
         <v>46</v>
       </c>
+      <c r="C43" t="s">
+        <v>33</v>
+      </c>
       <c r="D43" t="s">
         <v>33</v>
       </c>
       <c r="E43" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F43" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G43" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H43" t="s">
-        <v>102</v>
-      </c>
-      <c r="I43" t="s">
-        <v>9</v>
-      </c>
-      <c r="J43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>47</v>
       </c>
       <c r="B44" t="s">
         <v>47</v>
       </c>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
       <c r="D44" t="s">
         <v>33</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F44" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G44" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H44" t="s">
-        <v>102</v>
-      </c>
-      <c r="I44" t="s">
-        <v>9</v>
-      </c>
-      <c r="J44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>48</v>
       </c>
       <c r="B45" t="s">
         <v>48</v>
       </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
       <c r="D45" t="s">
         <v>33</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F45" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G45" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H45" t="s">
-        <v>102</v>
-      </c>
-      <c r="I45" t="s">
-        <v>9</v>
-      </c>
-      <c r="J45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>49</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
       </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
       <c r="D46" t="s">
         <v>33</v>
       </c>
       <c r="E46" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F46" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G46" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H46" t="s">
-        <v>102</v>
-      </c>
-      <c r="I46" t="s">
-        <v>9</v>
-      </c>
-      <c r="J46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>50</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
       </c>
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
       <c r="D47" t="s">
         <v>33</v>
       </c>
       <c r="E47" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G47" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H47" t="s">
-        <v>102</v>
-      </c>
-      <c r="I47" t="s">
-        <v>9</v>
-      </c>
-      <c r="J47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>51</v>
       </c>
       <c r="B48" t="s">
         <v>51</v>
       </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
       <c r="D48" t="s">
         <v>33</v>
       </c>
       <c r="E48" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F48" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G48" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H48" t="s">
-        <v>102</v>
-      </c>
-      <c r="I48" t="s">
-        <v>9</v>
-      </c>
-      <c r="J48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>52</v>
       </c>
       <c r="B49" t="s">
         <v>52</v>
       </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
       <c r="D49" t="s">
         <v>33</v>
       </c>
       <c r="E49" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F49" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G49" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H49" t="s">
-        <v>102</v>
-      </c>
-      <c r="I49" t="s">
-        <v>9</v>
-      </c>
-      <c r="J49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>53</v>
       </c>
       <c r="B50" t="s">
         <v>53</v>
       </c>
+      <c r="C50" t="s">
+        <v>33</v>
+      </c>
       <c r="D50" t="s">
         <v>33</v>
       </c>
       <c r="E50" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F50" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G50" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H50" t="s">
-        <v>102</v>
-      </c>
-      <c r="I50" t="s">
-        <v>9</v>
-      </c>
-      <c r="J50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>54</v>
       </c>
       <c r="B51" t="s">
         <v>54</v>
       </c>
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
       <c r="D51" t="s">
         <v>33</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F51" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G51" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="H51" t="s">
-        <v>102</v>
-      </c>
-      <c r="I51" t="s">
-        <v>9</v>
-      </c>
-      <c r="J51">
+        <v>9</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52" t="s">
+        <v>139</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" t="s">
+        <v>139</v>
+      </c>
+      <c r="E53" t="s">
+        <v>139</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" t="s">
+        <v>139</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55" t="s">
+        <v>139</v>
+      </c>
+      <c r="E55" t="s">
+        <v>139</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" t="s">
+        <v>139</v>
+      </c>
+      <c r="E56" t="s">
+        <v>139</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D57" t="s">
+        <v>139</v>
+      </c>
+      <c r="E57" t="s">
+        <v>139</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D58" t="s">
+        <v>139</v>
+      </c>
+      <c r="E58" t="s">
+        <v>139</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59" t="s">
+        <v>139</v>
+      </c>
+      <c r="E59" t="s">
+        <v>139</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" t="s">
+        <v>139</v>
+      </c>
+      <c r="E60" t="s">
+        <v>139</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D61" t="s">
+        <v>139</v>
+      </c>
+      <c r="E61" t="s">
+        <v>139</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" t="s">
+        <v>139</v>
+      </c>
+      <c r="I62">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some changes... still lots of work to do
</commit_message>
<xml_diff>
--- a/Auto/ASSETS.xlsx
+++ b/Auto/ASSETS.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trading\Auto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03547E63-FE64-4446-A14C-B28E5C3530B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F929E838-33FC-471F-BDCD-EBF421CB974F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7950" yWindow="2730" windowWidth="16875" windowHeight="10470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSETS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="157">
   <si>
     <t>symbol</t>
   </si>
@@ -286,9 +296,6 @@
     <t>Bitcoin</t>
   </si>
   <si>
-    <t>UnitedStated</t>
-  </si>
-  <si>
     <t>EBM</t>
   </si>
   <si>
@@ -443,6 +450,57 @@
   </si>
   <si>
     <t>ticker</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>ZAR</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>CHF</t>
+  </si>
+  <si>
+    <t>KRW</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Live Cattle</t>
+  </si>
+  <si>
+    <t>fututes</t>
+  </si>
+  <si>
+    <t>CME</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>ZO</t>
+  </si>
+  <si>
+    <t>Oats</t>
   </si>
 </sst>
 </file>
@@ -999,12 +1057,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I62" totalsRowShown="0">
-  <autoFilter ref="A1:I62" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I51">
-    <sortCondition ref="D2:D51"/>
-    <sortCondition ref="E2:E51"/>
-    <sortCondition ref="A2:A51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I64" totalsRowShown="0">
+  <autoFilter ref="A1:I64" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I53">
+    <sortCondition ref="D2:D53"/>
+    <sortCondition ref="E2:E53"/>
+    <sortCondition ref="A2:A53"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="symbol"/>
@@ -1318,29 +1376,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.53125" customWidth="1"/>
-    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.9296875" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" customWidth="1"/>
+    <col min="1" max="2" width="8.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" customWidth="1"/>
     <col min="6" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="9.59765625" customWidth="1"/>
-    <col min="9" max="9" width="10.53125" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1364,7 +1422,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1384,7 +1442,7 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
@@ -1393,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1413,7 +1471,7 @@
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
@@ -1422,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1442,7 +1500,7 @@
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" t="s">
         <v>9</v>
@@ -1451,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1471,7 +1529,7 @@
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
@@ -1480,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1500,7 +1558,7 @@
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" t="s">
         <v>9</v>
@@ -1509,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1529,7 +1587,7 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" t="s">
         <v>9</v>
@@ -1538,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -1558,7 +1616,7 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H8" t="s">
         <v>9</v>
@@ -1567,44 +1625,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
+        <v>150</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>153</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="H9" t="s">
         <v>9</v>
       </c>
       <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>63</v>
@@ -1613,27 +1671,27 @@
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
         <v>9</v>
       </c>
       <c r="I10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
         <v>63</v>
@@ -1642,27 +1700,27 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
       <c r="I11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
         <v>63</v>
@@ -1671,27 +1729,27 @@
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G12" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="H12" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="I12">
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
@@ -1703,7 +1761,7 @@
         <v>83</v>
       </c>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H13" t="s">
         <v>9</v>
@@ -1712,15 +1770,15 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D14" t="s">
         <v>63</v>
@@ -1732,24 +1790,24 @@
         <v>83</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="H14" t="s">
         <v>9</v>
       </c>
       <c r="I14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>154</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="D15" t="s">
         <v>63</v>
@@ -1758,27 +1816,24 @@
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="H15" t="s">
-        <v>93</v>
-      </c>
-      <c r="I15">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D16" t="s">
         <v>63</v>
@@ -1787,27 +1842,27 @@
         <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="H16" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
       <c r="I16">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
         <v>63</v>
@@ -1822,21 +1877,21 @@
         <v>69</v>
       </c>
       <c r="H17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>75</v>
+        <v>88</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
         <v>63</v>
@@ -1851,21 +1906,21 @@
         <v>69</v>
       </c>
       <c r="H18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>93</v>
       </c>
-      <c r="I18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" t="s">
-        <v>74</v>
+      <c r="B19" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
         <v>63</v>
@@ -1880,21 +1935,21 @@
         <v>69</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I19">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
         <v>63</v>
@@ -1903,27 +1958,27 @@
         <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H20" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="I20">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
         <v>63</v>
@@ -1932,27 +1987,27 @@
         <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H21" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="I21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
         <v>63</v>
@@ -1973,15 +2028,15 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
         <v>63</v>
@@ -1999,18 +2054,18 @@
         <v>9</v>
       </c>
       <c r="I23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>80</v>
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
         <v>63</v>
@@ -2019,27 +2074,27 @@
         <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="H24" t="s">
         <v>9</v>
       </c>
       <c r="I24">
-        <v>42000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -2048,27 +2103,27 @@
         <v>18</v>
       </c>
       <c r="F25" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H25" t="s">
         <v>9</v>
       </c>
       <c r="I25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
         <v>63</v>
@@ -2077,27 +2132,27 @@
         <v>18</v>
       </c>
       <c r="F26" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="G26" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="H26" t="s">
         <v>9</v>
       </c>
       <c r="I26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
         <v>63</v>
@@ -2106,27 +2161,27 @@
         <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G27" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="H27" t="s">
         <v>9</v>
       </c>
       <c r="I27">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D28" t="s">
         <v>63</v>
@@ -2135,27 +2190,27 @@
         <v>18</v>
       </c>
       <c r="F28" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G28" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="H28" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>112</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
         <v>63</v>
@@ -2163,25 +2218,28 @@
       <c r="E29" t="s">
         <v>18</v>
       </c>
+      <c r="F29" t="s">
+        <v>19</v>
+      </c>
       <c r="G29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H29" t="s">
         <v>9</v>
       </c>
-      <c r="I29" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C30" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
         <v>63</v>
@@ -2189,80 +2247,77 @@
       <c r="E30" t="s">
         <v>18</v>
       </c>
+      <c r="F30" t="s">
+        <v>19</v>
+      </c>
       <c r="G30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H30" t="s">
         <v>9</v>
       </c>
       <c r="I30" s="2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" t="s">
+        <v>101</v>
+      </c>
+      <c r="H31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>101</v>
+      </c>
+      <c r="H32" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>32</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H31" t="s">
-        <v>9</v>
-      </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" t="s">
-        <v>34</v>
-      </c>
-      <c r="G32" t="s">
-        <v>102</v>
-      </c>
-      <c r="H32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" t="s">
-        <v>36</v>
       </c>
       <c r="C33" t="s">
         <v>33</v>
@@ -2277,7 +2332,7 @@
         <v>34</v>
       </c>
       <c r="G33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H33" t="s">
         <v>9</v>
@@ -2286,12 +2341,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
         <v>33</v>
@@ -2306,7 +2361,7 @@
         <v>34</v>
       </c>
       <c r="G34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H34" t="s">
         <v>9</v>
@@ -2315,12 +2370,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
         <v>33</v>
@@ -2335,7 +2390,7 @@
         <v>34</v>
       </c>
       <c r="G35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H35" t="s">
         <v>9</v>
@@ -2344,12 +2399,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
         <v>33</v>
@@ -2364,7 +2419,7 @@
         <v>34</v>
       </c>
       <c r="G36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H36" t="s">
         <v>9</v>
@@ -2373,12 +2428,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
         <v>33</v>
@@ -2393,7 +2448,7 @@
         <v>34</v>
       </c>
       <c r="G37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H37" t="s">
         <v>9</v>
@@ -2402,12 +2457,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
         <v>33</v>
@@ -2422,7 +2477,7 @@
         <v>34</v>
       </c>
       <c r="G38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H38" t="s">
         <v>9</v>
@@ -2431,12 +2486,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
         <v>33</v>
@@ -2451,7 +2506,7 @@
         <v>34</v>
       </c>
       <c r="G39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H39" t="s">
         <v>9</v>
@@ -2460,12 +2515,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
         <v>33</v>
@@ -2480,7 +2535,7 @@
         <v>34</v>
       </c>
       <c r="G40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H40" t="s">
         <v>9</v>
@@ -2489,12 +2544,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
         <v>33</v>
@@ -2509,7 +2564,7 @@
         <v>34</v>
       </c>
       <c r="G41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H41" t="s">
         <v>9</v>
@@ -2518,12 +2573,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C42" t="s">
         <v>33</v>
@@ -2538,7 +2593,7 @@
         <v>34</v>
       </c>
       <c r="G42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H42" t="s">
         <v>9</v>
@@ -2547,12 +2602,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C43" t="s">
         <v>33</v>
@@ -2567,7 +2622,7 @@
         <v>34</v>
       </c>
       <c r="G43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H43" t="s">
         <v>9</v>
@@ -2576,12 +2631,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
         <v>33</v>
@@ -2596,7 +2651,7 @@
         <v>34</v>
       </c>
       <c r="G44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H44" t="s">
         <v>9</v>
@@ -2605,12 +2660,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
         <v>33</v>
@@ -2625,7 +2680,7 @@
         <v>34</v>
       </c>
       <c r="G45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H45" t="s">
         <v>9</v>
@@ -2634,12 +2689,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
         <v>33</v>
@@ -2654,7 +2709,7 @@
         <v>34</v>
       </c>
       <c r="G46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H46" t="s">
         <v>9</v>
@@ -2663,12 +2718,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
         <v>33</v>
@@ -2683,7 +2738,7 @@
         <v>34</v>
       </c>
       <c r="G47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H47" t="s">
         <v>9</v>
@@ -2692,12 +2747,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C48" t="s">
         <v>33</v>
@@ -2712,7 +2767,7 @@
         <v>34</v>
       </c>
       <c r="G48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H48" t="s">
         <v>9</v>
@@ -2721,12 +2776,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C49" t="s">
         <v>33</v>
@@ -2741,7 +2796,7 @@
         <v>34</v>
       </c>
       <c r="G49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H49" t="s">
         <v>9</v>
@@ -2750,12 +2805,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
         <v>33</v>
@@ -2770,7 +2825,7 @@
         <v>34</v>
       </c>
       <c r="G50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H50" t="s">
         <v>9</v>
@@ -2779,12 +2834,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
         <v>33</v>
@@ -2799,7 +2854,7 @@
         <v>34</v>
       </c>
       <c r="G51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H51" t="s">
         <v>9</v>
@@ -2808,223 +2863,314 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" t="s">
+        <v>34</v>
+      </c>
+      <c r="G52" t="s">
+        <v>101</v>
+      </c>
+      <c r="H52" t="s">
+        <v>9</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" t="s">
+        <v>101</v>
+      </c>
+      <c r="H53" t="s">
+        <v>9</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D54" t="s">
+        <v>138</v>
+      </c>
+      <c r="E54" t="s">
+        <v>138</v>
+      </c>
+      <c r="H54" t="s">
+        <v>140</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B55" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" t="s">
+        <v>138</v>
+      </c>
+      <c r="E55" t="s">
+        <v>138</v>
+      </c>
+      <c r="H55" t="s">
+        <v>141</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E52" t="s">
-        <v>139</v>
-      </c>
-      <c r="I52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>118</v>
-      </c>
-      <c r="B53" s="1" t="s">
+      <c r="D56" t="s">
+        <v>138</v>
+      </c>
+      <c r="E56" t="s">
+        <v>138</v>
+      </c>
+      <c r="H56" t="s">
+        <v>92</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D57" t="s">
+        <v>138</v>
+      </c>
+      <c r="E57" t="s">
+        <v>138</v>
+      </c>
+      <c r="H57" t="s">
+        <v>142</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D58" t="s">
+        <v>138</v>
+      </c>
+      <c r="E58" t="s">
+        <v>138</v>
+      </c>
+      <c r="H58" t="s">
+        <v>143</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D59" t="s">
+        <v>138</v>
+      </c>
+      <c r="E59" t="s">
+        <v>138</v>
+      </c>
+      <c r="H59" t="s">
+        <v>144</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D60" t="s">
+        <v>138</v>
+      </c>
+      <c r="E60" t="s">
+        <v>138</v>
+      </c>
+      <c r="H60" t="s">
+        <v>145</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" t="s">
+        <v>138</v>
+      </c>
+      <c r="E61" t="s">
+        <v>138</v>
+      </c>
+      <c r="H61" t="s">
+        <v>146</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62" t="s">
+        <v>138</v>
+      </c>
+      <c r="E62" t="s">
+        <v>138</v>
+      </c>
+      <c r="H62" t="s">
+        <v>147</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D53" t="s">
-        <v>139</v>
-      </c>
-      <c r="E53" t="s">
-        <v>139</v>
-      </c>
-      <c r="I53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>119</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D54" t="s">
-        <v>139</v>
-      </c>
-      <c r="E54" t="s">
-        <v>139</v>
-      </c>
-      <c r="I54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>120</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D55" t="s">
-        <v>139</v>
-      </c>
-      <c r="E55" t="s">
-        <v>139</v>
-      </c>
-      <c r="I55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D56" t="s">
-        <v>139</v>
-      </c>
-      <c r="E56" t="s">
-        <v>139</v>
-      </c>
-      <c r="I56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>122</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D57" t="s">
-        <v>139</v>
-      </c>
-      <c r="E57" t="s">
-        <v>139</v>
-      </c>
-      <c r="I57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>123</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D58" t="s">
-        <v>139</v>
-      </c>
-      <c r="E58" t="s">
-        <v>139</v>
-      </c>
-      <c r="I58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>124</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D59" t="s">
-        <v>139</v>
-      </c>
-      <c r="E59" t="s">
-        <v>139</v>
-      </c>
-      <c r="I59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>125</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D60" t="s">
-        <v>139</v>
-      </c>
-      <c r="E60" t="s">
-        <v>139</v>
-      </c>
-      <c r="I60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+      <c r="D63" t="s">
+        <v>138</v>
+      </c>
+      <c r="E63" t="s">
+        <v>138</v>
+      </c>
+      <c r="H63" t="s">
+        <v>148</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D61" t="s">
-        <v>139</v>
-      </c>
-      <c r="E61" t="s">
-        <v>139</v>
-      </c>
-      <c r="I61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="D64" t="s">
         <v>138</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="E64" t="s">
         <v>138</v>
       </c>
-      <c r="D62" t="s">
-        <v>139</v>
-      </c>
-      <c r="E62" t="s">
-        <v>139</v>
-      </c>
-      <c r="I62">
+      <c r="H64" t="s">
+        <v>149</v>
+      </c>
+      <c r="I64">
         <v>1</v>
       </c>
     </row>

</xml_diff>